<commit_message>
Deploying to gh-pages from @ LAPKB/Pmetrics_rust@55d53dc73c13bb1ed4f97c2f3b8b2565355a337e 🚀
</commit_message>
<xml_diff>
--- a/articles/Data/PM_result.xlsx
+++ b/articles/Data/PM_result.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10507"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11109"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mneely/LAPK/Development/PM_manual/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mneely/Library/CloudStorage/OneDrive-CHILDRENSHOSPITALLOSANGELES/Documents/LAPK/Development/Pmetrics_rust/vignettes/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DE7A391-43DD-2C46-B29E-7ABD393D9DD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E76C5976-C0ED-F54F-9FBF-3A6E526C6B5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="1" xr2:uid="{079C664A-AD6E-D640-A7A9-23C2474CF6FC}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="198">
   <si>
     <t>Objects</t>
   </si>
@@ -549,9 +549,6 @@
     <t>\$post (class: PM_post)</t>
   </si>
   <si>
-    <t>\$npdata (class: NPAG, list); \$itdata (class: IT2B, list)</t>
-  </si>
-  <si>
     <t>\$new</t>
   </si>
   <si>
@@ -574,6 +571,66 @@
   </si>
   <si>
     <t>Alternative method to summarize objects, e.g. PM_result$summary("final") = PM_result$final$summary() = summary(PM_result$final)</t>
+  </si>
+  <si>
+    <t>\$cens</t>
+  </si>
+  <si>
+    <t>\$errfile</t>
+  </si>
+  <si>
+    <t>Name of error file if it exists</t>
+  </si>
+  <si>
+    <t>\$success</t>
+  </si>
+  <si>
+    <t>Boolean for successful run</t>
+  </si>
+  <si>
+    <t>\$fit</t>
+  </si>
+  <si>
+    <t>Fit data using the model in the PM_result object</t>
+  </si>
+  <si>
+    <t>Calculate auc by supplying a src, e.g. PM_result$auc("op")</t>
+  </si>
+  <si>
+    <t>\$report</t>
+  </si>
+  <si>
+    <t>Regenerate the report</t>
+  </si>
+  <si>
+    <t>\$sim</t>
+  </si>
+  <si>
+    <t>Simulate using the model in the PM_result object</t>
+  </si>
+  <si>
+    <t>\$save</t>
+  </si>
+  <si>
+    <t>Save the PM_result object</t>
+  </si>
+  <si>
+    <t>\$validate</t>
+  </si>
+  <si>
+    <t>Validate by simuation to create VPC or NPDE as a PM_valid object</t>
+  </si>
+  <si>
+    <t>\$step</t>
+  </si>
+  <si>
+    <t>Stepwise forward/backward linear regression between covariates and model parameter values</t>
+  </si>
+  <si>
+    <t>\$opt</t>
+  </si>
+  <si>
+    <t>Optimal sampling to create a PM_opt object</t>
   </si>
 </sst>
 </file>
@@ -629,9 +686,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -669,7 +726,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -775,7 +832,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -917,7 +974,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -925,10 +982,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{088BC2A6-70E9-BE41-9D06-0C982EE54A93}">
-  <dimension ref="A1:D74"/>
+  <dimension ref="A1:D76"/>
   <sheetViews>
-    <sheetView zoomScale="142" zoomScaleNormal="142" workbookViewId="0">
-      <selection activeCell="D75" sqref="D75"/>
+    <sheetView topLeftCell="A56" zoomScale="142" zoomScaleNormal="142" workbookViewId="0">
+      <selection activeCell="A77" sqref="A77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -982,525 +1039,522 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>83</v>
-      </c>
-      <c r="D5" t="s">
-        <v>6</v>
+        <v>178</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
-        <v>86</v>
+        <v>85</v>
+      </c>
+      <c r="D8" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
-        <v>87</v>
-      </c>
-      <c r="D9" t="s">
-        <v>9</v>
+        <v>86</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D13" t="s">
-        <v>92</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D14" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
+        <v>93</v>
+      </c>
+      <c r="D15" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
         <v>145</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D16" t="s">
         <v>146</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C16" t="s">
-        <v>147</v>
-      </c>
-      <c r="D16" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C17" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D17" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C18" t="s">
+        <v>148</v>
+      </c>
+      <c r="D18" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C19" t="s">
         <v>149</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D19" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
         <v>165</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B22" t="s">
         <v>95</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D22" t="s">
         <v>153</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B22" t="s">
-        <v>97</v>
-      </c>
-      <c r="D22" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D23" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D25" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D26" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D27" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D28" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D29" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
+        <v>104</v>
+      </c>
+      <c r="D30" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B31" t="s">
         <v>105</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D31" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D31" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D32" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D33" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D34" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D35" t="s">
         <v>75</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B35" t="s">
-        <v>106</v>
-      </c>
-      <c r="D35" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D36" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D37" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D38" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D39" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D40" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D41" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B42" t="s">
+        <v>112</v>
+      </c>
+      <c r="D42" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B43" t="s">
         <v>145</v>
       </c>
-      <c r="D42" t="s">
+      <c r="D43" t="s">
         <v>151</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C43" t="s">
-        <v>147</v>
-      </c>
-      <c r="D43" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C44" t="s">
+        <v>147</v>
+      </c>
+      <c r="D44" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C45" t="s">
         <v>148</v>
       </c>
-      <c r="D44" t="s">
+      <c r="D45" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
         <v>166</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B46" t="s">
         <v>113</v>
       </c>
-      <c r="D45" t="s">
+      <c r="D46" t="s">
         <v>31</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B46" t="s">
-        <v>114</v>
-      </c>
-      <c r="D46" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D47" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B48" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D48" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B49" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D49" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D50" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B51" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D51" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B52" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D52" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B53" t="s">
+        <v>120</v>
+      </c>
+      <c r="D53" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B54" t="s">
         <v>145</v>
       </c>
-      <c r="D53" t="s">
+      <c r="D54" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C54" t="s">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C55" t="s">
         <v>147</v>
       </c>
-      <c r="D54" t="s">
+      <c r="D55" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
         <v>167</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B56" t="s">
         <v>80</v>
       </c>
-      <c r="D55" t="s">
+      <c r="D56" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B56" t="s">
-        <v>81</v>
-      </c>
-      <c r="D56" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B57" t="s">
-        <v>41</v>
+        <v>81</v>
       </c>
       <c r="D57" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B58" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D58" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B59" t="s">
-        <v>85</v>
+        <v>43</v>
       </c>
       <c r="D59" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B60" t="s">
+        <v>85</v>
+      </c>
+      <c r="D60" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B61" t="s">
         <v>145</v>
       </c>
-      <c r="D60" t="s">
+      <c r="D61" t="s">
         <v>151</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C61" t="s">
-        <v>147</v>
-      </c>
-      <c r="D61" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C62" t="s">
+        <v>147</v>
+      </c>
+      <c r="D62" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C63" t="s">
         <v>148</v>
       </c>
-      <c r="D62" t="s">
+      <c r="D63" t="s">
         <v>159</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A64" t="s">
-        <v>168</v>
-      </c>
-      <c r="B64" t="s">
-        <v>80</v>
-      </c>
-      <c r="D64" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B65" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D65" t="s">
-        <v>76</v>
+        <v>3</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
+        <v>169</v>
+      </c>
+      <c r="B66" t="s">
+        <v>81</v>
+      </c>
+      <c r="D66" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
         <v>161</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B67" t="s">
         <v>85</v>
       </c>
-      <c r="D66" t="s">
+      <c r="D67" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B67" t="s">
-        <v>83</v>
-      </c>
-      <c r="D67" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B68" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D68" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B69" t="s">
+        <v>86</v>
+      </c>
+      <c r="D69" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B70" t="s">
         <v>87</v>
       </c>
-      <c r="D69" t="s">
+      <c r="D70" t="s">
         <v>51</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C70" t="s">
-        <v>149</v>
-      </c>
-      <c r="D70" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C71" t="s">
+        <v>149</v>
+      </c>
+      <c r="D71" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C72" t="s">
+        <v>173</v>
+      </c>
+      <c r="D72" t="s">
         <v>174</v>
-      </c>
-      <c r="D71" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A72" t="s">
-        <v>170</v>
-      </c>
-      <c r="D72" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
@@ -1511,7 +1565,7 @@
         <v>54</v>
       </c>
       <c r="D73" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
@@ -1522,7 +1576,23 @@
         <v>54</v>
       </c>
       <c r="D74" t="s">
-        <v>177</v>
+        <v>176</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>179</v>
+      </c>
+      <c r="B75" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>181</v>
+      </c>
+      <c r="B76" t="s">
+        <v>182</v>
       </c>
     </row>
   </sheetData>
@@ -1533,10 +1603,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{621E75FF-8B74-2448-8200-4AD633345001}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1555,10 +1625,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>170</v>
+      </c>
+      <c r="B2" t="s">
         <v>171</v>
-      </c>
-      <c r="B2" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -1566,7 +1636,7 @@
         <v>147</v>
       </c>
       <c r="B3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -1574,7 +1644,71 @@
         <v>148</v>
       </c>
       <c r="B4" t="s">
-        <v>178</v>
+        <v>177</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>183</v>
+      </c>
+      <c r="B5" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>149</v>
+      </c>
+      <c r="B6" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>186</v>
+      </c>
+      <c r="B7" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>188</v>
+      </c>
+      <c r="B8" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>190</v>
+      </c>
+      <c r="B9" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>192</v>
+      </c>
+      <c r="B10" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>194</v>
+      </c>
+      <c r="B11" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>196</v>
+      </c>
+      <c r="B12" t="s">
+        <v>197</v>
       </c>
     </row>
   </sheetData>

</xml_diff>